<commit_message>
Update £TED following acquisition by Authentic Brands Group
</commit_message>
<xml_diff>
--- a/£TED.xlsx
+++ b/£TED.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FE6E07-0A99-4A3C-944B-20ADF6F488B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769F2501-F00A-A349-94E9-AB96B334F11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{CF719F56-9BF4-487E-BB92-90A9ADCC368F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="138">
   <si>
     <t>Stock Snapshot</t>
   </si>
@@ -471,6 +481,9 @@
   </si>
   <si>
     <t>Inventory/Revenue</t>
+  </si>
+  <si>
+    <t>Ted Baker is delisted from the London Stock Exchange following takeover by Authentic Brands Group</t>
   </si>
 </sst>
 </file>
@@ -686,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -764,18 +777,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,10 +786,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -797,6 +798,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1181,54 +1195,54 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:24" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:24" ht="14" x14ac:dyDescent="0.15">
       <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="53" t="s">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="55"/>
-      <c r="H5" s="53" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="H5" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="54"/>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="55"/>
-      <c r="U5" s="53" t="s">
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="51"/>
+      <c r="U5" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="V5" s="54"/>
-      <c r="W5" s="54"/>
-      <c r="X5" s="55"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="V5" s="50"/>
+      <c r="W5" s="50"/>
+      <c r="X5" s="51"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1237,10 +1251,10 @@
       </c>
       <c r="D6" s="3"/>
       <c r="H6" s="18">
-        <v>44774</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>135</v>
+        <v>44835</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>137</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
@@ -1258,7 +1272,7 @@
       <c r="W6" s="14"/>
       <c r="X6" s="15"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1286,7 +1300,7 @@
       <c r="W7" s="14"/>
       <c r="X7" s="15"/>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1313,7 +1327,7 @@
       <c r="W8" s="14"/>
       <c r="X8" s="15"/>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1323,12 +1337,8 @@
       <c r="D9" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="18">
-        <v>43922</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>74</v>
-      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
@@ -1345,7 +1355,7 @@
       <c r="W9" s="14"/>
       <c r="X9" s="15"/>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1353,9 +1363,11 @@
       <c r="D10" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="19" t="s">
-        <v>73</v>
+      <c r="H10" s="18">
+        <v>44774</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
@@ -1373,7 +1385,7 @@
       <c r="W10" s="14"/>
       <c r="X10" s="15"/>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1414,7 @@
       <c r="W11" s="14"/>
       <c r="X11" s="15"/>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1429,12 +1441,12 @@
       <c r="W12" s="14"/>
       <c r="X12" s="15"/>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
       <c r="H13" s="18">
-        <v>43525</v>
+        <v>43922</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -1452,12 +1464,10 @@
       <c r="W13" s="14"/>
       <c r="X13" s="15"/>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="H14" s="18">
-        <v>43435</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>54</v>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="H14" s="10"/>
+      <c r="I14" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
@@ -1475,12 +1485,12 @@
       <c r="W14" s="14"/>
       <c r="X14" s="15"/>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="B15" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="H15" s="10"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1499,14 +1509,14 @@
       <c r="W15" s="14"/>
       <c r="X15" s="15"/>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.15">
       <c r="B16" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="52"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1528,16 +1538,20 @@
       <c r="W16" s="16"/>
       <c r="X16" s="17"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B17" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="14"/>
+      <c r="D17" s="53"/>
+      <c r="H17" s="18">
+        <v>43525</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
@@ -1549,12 +1563,16 @@
       <c r="R17" s="15"/>
       <c r="U17" s="20"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B18" s="24"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="14"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="H18" s="18">
+        <v>43435</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
       <c r="L18" s="14"/>
@@ -1566,10 +1584,10 @@
       <c r="R18" s="15"/>
       <c r="U18" s="20"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B19" s="25"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="59"/>
       <c r="H19" s="10"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1582,7 +1600,7 @@
       <c r="Q19" s="14"/>
       <c r="R19" s="15"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.15">
       <c r="H20" s="10"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1595,7 +1613,7 @@
       <c r="Q20" s="14"/>
       <c r="R20" s="15"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.15">
       <c r="H21" s="10"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -1608,12 +1626,12 @@
       <c r="Q21" s="14"/>
       <c r="R21" s="15"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="53" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B22" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
       <c r="H22" s="10"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -1626,14 +1644,14 @@
       <c r="Q22" s="14"/>
       <c r="R22" s="15"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="53"/>
       <c r="H23" s="10"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1646,17 +1664,17 @@
       <c r="Q23" s="14"/>
       <c r="R23" s="15"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="51">
+      <c r="C24" s="52">
         <v>1987</v>
       </c>
-      <c r="D24" s="52"/>
+      <c r="D24" s="53"/>
       <c r="H24" s="10"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1669,14 +1687,14 @@
       <c r="Q24" s="14"/>
       <c r="R24" s="15"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="51">
+      <c r="C25" s="52">
         <v>85</v>
       </c>
-      <c r="D25" s="52"/>
+      <c r="D25" s="53"/>
       <c r="H25" s="10"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -1689,15 +1707,15 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="15"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B26" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="56">
         <f>'Financial Model'!T48</f>
         <v>103.071</v>
       </c>
-      <c r="D26" s="50"/>
+      <c r="D26" s="57"/>
       <c r="H26" s="10"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -1710,10 +1728,10 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="15"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B27" s="10"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="53"/>
       <c r="H27" s="10"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -1726,14 +1744,14 @@
       <c r="Q27" s="14"/>
       <c r="R27" s="15"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B28" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C28" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="52"/>
+      <c r="D28" s="53"/>
       <c r="H28" s="10"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -1746,14 +1764,14 @@
       <c r="Q28" s="14"/>
       <c r="R28" s="15"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B29" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="59"/>
+      <c r="D29" s="55"/>
       <c r="H29" s="10"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -1766,7 +1784,7 @@
       <c r="Q29" s="14"/>
       <c r="R29" s="15"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="H30" s="10"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -1779,7 +1797,7 @@
       <c r="Q30" s="14"/>
       <c r="R30" s="15"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="H31" s="10"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -1792,12 +1810,12 @@
       <c r="Q31" s="14"/>
       <c r="R31" s="15"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B32" s="53" t="s">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="B32" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="51"/>
       <c r="H32" s="10"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -1810,12 +1828,12 @@
       <c r="Q32" s="14"/>
       <c r="R32" s="15"/>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B33" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="53"/>
       <c r="H33" s="10"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -1828,12 +1846,12 @@
       <c r="Q33" s="14"/>
       <c r="R33" s="15"/>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
       <c r="H34" s="10"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1846,12 +1864,12 @@
       <c r="Q34" s="14"/>
       <c r="R34" s="15"/>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B35" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="53"/>
       <c r="H35" s="10"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -1864,12 +1882,12 @@
       <c r="Q35" s="14"/>
       <c r="R35" s="15"/>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B36" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
       <c r="H36" s="10"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -1882,10 +1900,10 @@
       <c r="Q36" s="14"/>
       <c r="R36" s="15"/>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B37" s="10"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
       <c r="H37" s="10"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -1898,10 +1916,10 @@
       <c r="Q37" s="14"/>
       <c r="R37" s="15"/>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B38" s="10"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="53"/>
       <c r="H38" s="11"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
@@ -1914,15 +1932,23 @@
       <c r="Q38" s="16"/>
       <c r="R38" s="17"/>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B39" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="59"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="U5:X5"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
@@ -1939,21 +1965,14 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{FB479492-F5F1-324E-B8E6-A88CE3D1033A}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{58A051F3-58D6-4647-9350-FA96554C3CB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1968,26 +1987,26 @@
       <selection pane="bottomRight" activeCell="S76" sqref="S76:T76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="9.140625" style="46"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.140625" style="46"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.140625" style="46"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="46"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="9.140625" style="46"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.140625" style="46"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.1640625" style="46"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="9.1640625" style="46"/>
+    <col min="7" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="9.1640625" style="46"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="9.1640625" style="46"/>
+    <col min="11" max="11" width="9.1640625" style="1"/>
+    <col min="12" max="12" width="9.1640625" style="46"/>
+    <col min="13" max="13" width="9.1640625" style="1"/>
+    <col min="14" max="14" width="9.1640625" style="46"/>
+    <col min="15" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:32" s="13" customFormat="1" x14ac:dyDescent="0.15">
       <c r="C1" s="13" t="s">
         <v>26</v>
       </c>
@@ -2076,7 +2095,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:32" s="26" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B2" s="27"/>
       <c r="D2" s="43"/>
       <c r="F2" s="43"/>
@@ -2091,7 +2110,7 @@
         <v>44590</v>
       </c>
     </row>
-    <row r="3" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="39" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2127,7 @@
         <v>168.13</v>
       </c>
     </row>
-    <row r="4" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="39" t="s">
         <v>102</v>
       </c>
@@ -2125,7 +2144,7 @@
         <v>133.80000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="39" t="s">
         <v>103</v>
       </c>
@@ -2142,7 +2161,7 @@
         <v>111.2</v>
       </c>
     </row>
-    <row r="6" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:32" s="40" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="39" t="s">
         <v>104</v>
       </c>
@@ -2159,7 +2178,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="7" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="7" t="s">
         <v>76</v>
       </c>
@@ -2178,7 +2197,7 @@
         <v>428.33</v>
       </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>77</v>
       </c>
@@ -2189,7 +2208,7 @@
         <v>190.66300000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="7" t="s">
         <v>78</v>
       </c>
@@ -2208,7 +2227,7 @@
         <v>237.66699999999997</v>
       </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>79</v>
       </c>
@@ -2219,7 +2238,7 @@
         <v>187.07400000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
@@ -2230,7 +2249,7 @@
         <v>95.864999999999995</v>
       </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
@@ -2241,7 +2260,7 @@
         <v>10.797000000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:32" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="7" t="s">
         <v>82</v>
       </c>
@@ -2260,7 +2279,7 @@
         <v>-34.475000000000037</v>
       </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>83</v>
       </c>
@@ -2271,7 +2290,7 @@
         <v>-1.27</v>
       </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>84</v>
       </c>
@@ -2282,7 +2301,7 @@
         <v>0.25900000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>85</v>
       </c>
@@ -2293,7 +2312,7 @@
         <v>8.4740000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>86</v>
       </c>
@@ -2306,7 +2325,7 @@
         <v>-43.960000000000036</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>87</v>
       </c>
@@ -2317,7 +2336,7 @@
         <v>-8.4659999999999993</v>
       </c>
     </row>
-    <row r="19" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
         <v>88</v>
       </c>
@@ -2336,7 +2355,7 @@
         <v>-35.494000000000035</v>
       </c>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>89</v>
       </c>
@@ -2349,7 +2368,7 @@
         <v>-0.19226406307158311</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -2360,7 +2379,7 @@
         <v>184.61068299999999</v>
       </c>
     </row>
-    <row r="23" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="7" t="s">
         <v>90</v>
       </c>
@@ -2375,7 +2394,7 @@
         <v>0.20588400900900905</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>91</v>
       </c>
@@ -2386,7 +2405,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>93</v>
       </c>
@@ -2399,7 +2418,7 @@
         <v>0.55486890948567691</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>94</v>
       </c>
@@ -2412,7 +2431,7 @@
         <v>-8.0487007680993719E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
@@ -2425,7 +2444,7 @@
         <v>-8.2866014521513875E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
         <v>96</v>
       </c>
@@ -2438,22 +2457,22 @@
         <v>0.19258416742493159</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.15">
       <c r="S30" s="32"/>
       <c r="T30" s="32"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.15">
       <c r="S31" s="32"/>
       <c r="T31" s="32"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B32" s="33" t="s">
         <v>98</v>
       </c>
       <c r="S32" s="32"/>
       <c r="T32" s="32"/>
     </row>
-    <row r="33" spans="2:20" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="38" t="s">
         <v>99</v>
       </c>
@@ -2470,7 +2489,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:20" s="38" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" s="38" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B34" s="38" t="s">
         <v>100</v>
       </c>
@@ -2487,7 +2506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>101</v>
       </c>
@@ -2498,12 +2517,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B38" s="33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>105</v>
       </c>
@@ -2514,7 +2533,7 @@
         <v>28.420999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>106</v>
       </c>
@@ -2525,7 +2544,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>107</v>
       </c>
@@ -2536,7 +2555,7 @@
         <v>63.518999999999998</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>108</v>
       </c>
@@ -2547,7 +2566,7 @@
         <v>2.4209999999999998</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>109</v>
       </c>
@@ -2558,7 +2577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>113</v>
       </c>
@@ -2569,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
@@ -2580,7 +2599,7 @@
         <v>35.186999999999998</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>111</v>
       </c>
@@ -2591,7 +2610,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>112</v>
       </c>
@@ -2604,7 +2623,7 @@
         <v>159.83199999999999</v>
       </c>
     </row>
-    <row r="48" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B48" s="7" t="s">
         <v>114</v>
       </c>
@@ -2621,7 +2640,7 @@
         <v>103.071</v>
       </c>
     </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>115</v>
       </c>
@@ -2632,7 +2651,7 @@
         <v>56.66</v>
       </c>
     </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>116</v>
       </c>
@@ -2643,7 +2662,7 @@
         <v>4.5049999999999999</v>
       </c>
     </row>
-    <row r="51" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
         <v>117</v>
       </c>
@@ -2654,7 +2673,7 @@
         <v>1.2929999999999999</v>
       </c>
     </row>
-    <row r="52" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B52" s="7" t="s">
         <v>4</v>
       </c>
@@ -2671,7 +2690,7 @@
         <v>14.515000000000001</v>
       </c>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>118</v>
       </c>
@@ -2684,10 +2703,10 @@
         <v>339.87599999999998</v>
       </c>
     </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.15">
       <c r="S54" s="34"/>
     </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>119</v>
       </c>
@@ -2698,7 +2717,7 @@
         <v>76.893000000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B56" s="7" t="s">
         <v>120</v>
       </c>
@@ -2715,7 +2734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B57" s="7" t="s">
         <v>121</v>
       </c>
@@ -2732,7 +2751,7 @@
         <v>3.4169999999999998</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
@@ -2743,7 +2762,7 @@
         <v>3.028</v>
       </c>
     </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>123</v>
       </c>
@@ -2754,7 +2773,7 @@
         <v>43.128999999999998</v>
       </c>
     </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>124</v>
       </c>
@@ -2765,7 +2784,7 @@
         <v>0.19900000000000001</v>
       </c>
     </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
         <v>125</v>
       </c>
@@ -2776,7 +2795,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>126</v>
       </c>
@@ -2789,7 +2808,7 @@
         <v>134.74100000000001</v>
       </c>
     </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>124</v>
       </c>
@@ -2800,7 +2819,7 @@
         <v>2.8620000000000001</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
         <v>123</v>
       </c>
@@ -2811,7 +2830,7 @@
         <v>81.805000000000007</v>
       </c>
     </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
         <v>110</v>
       </c>
@@ -2822,7 +2841,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>127</v>
       </c>
@@ -2835,10 +2854,10 @@
         <v>219.48800000000003</v>
       </c>
     </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:20" x14ac:dyDescent="0.15">
       <c r="S67" s="34"/>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B68" s="1" t="s">
         <v>128</v>
       </c>
@@ -2849,7 +2868,7 @@
         <v>120.38800000000001</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>129</v>
       </c>
@@ -2862,10 +2881,10 @@
         <v>339.87600000000003</v>
       </c>
     </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:20" x14ac:dyDescent="0.15">
       <c r="S70" s="34"/>
     </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B71" s="1" t="s">
         <v>132</v>
       </c>
@@ -2878,7 +2897,7 @@
         <v>120.38799999999995</v>
       </c>
     </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B72" s="1" t="s">
         <v>133</v>
       </c>
@@ -2891,7 +2910,7 @@
         <v>0.65211827421709911</v>
       </c>
     </row>
-    <row r="74" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:20" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B74" s="7" t="s">
         <v>134</v>
       </c>
@@ -2906,7 +2925,7 @@
         <v>0.17328795191694746</v>
       </c>
     </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:20" x14ac:dyDescent="0.15">
       <c r="B76" s="1" t="s">
         <v>136</v>
       </c>

</xml_diff>